<commit_message>
post 14 - 완료 및 정리
</commit_message>
<xml_diff>
--- a/Post14/result-2201010B-openpyxl_part1.xlsx
+++ b/Post14/result-2201010B-openpyxl_part1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="제1작업" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="제1작업" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="급여">제1작업!$H$5:$H$12</definedName>
@@ -357,7 +357,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -372,13 +372,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -670,7 +670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1135,6 +1135,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>